<commit_message>
Roh-Erz-Blöcke und Material-Items vervollständigt (Tags)
</commit_message>
<xml_diff>
--- a/Versandordner/Assets (technisch)/Liste Metallblockwerte.xlsx
+++ b/Versandordner/Assets (technisch)/Liste Metallblockwerte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="330">
   <si>
     <t>BLOCK</t>
   </si>
@@ -837,6 +837,183 @@
   </si>
   <si>
     <t>forge:tiny_dusts/redstone_alloy</t>
+  </si>
+  <si>
+    <t>crushed_stone</t>
+  </si>
+  <si>
+    <t>crushed_zinc_ore</t>
+  </si>
+  <si>
+    <t>purified_crushed_zinc_ore</t>
+  </si>
+  <si>
+    <t>crushed_lead_ore</t>
+  </si>
+  <si>
+    <t>purified_crushed_lead_ore</t>
+  </si>
+  <si>
+    <t>crushed_gold_ore</t>
+  </si>
+  <si>
+    <t>purified_crushed_gold_ore</t>
+  </si>
+  <si>
+    <t>crushed_nether_gold_ore</t>
+  </si>
+  <si>
+    <t>crushed_nickel_ore</t>
+  </si>
+  <si>
+    <t>purified_crushed_nickel_ore</t>
+  </si>
+  <si>
+    <t>crushed_palladium_ore</t>
+  </si>
+  <si>
+    <t>purified_crushed_palladium_ore</t>
+  </si>
+  <si>
+    <t>crushed_tin_ore</t>
+  </si>
+  <si>
+    <t>purified_crushed_tin_ore</t>
+  </si>
+  <si>
+    <t>crushed_iron_ore</t>
+  </si>
+  <si>
+    <t>purified_crushed_iron_ore</t>
+  </si>
+  <si>
+    <t>crushed_copper_ore</t>
+  </si>
+  <si>
+    <t>purified_crushed_copper_ore</t>
+  </si>
+  <si>
+    <t>crushed_silver_ore</t>
+  </si>
+  <si>
+    <t>purified_crushed_silver_ore</t>
+  </si>
+  <si>
+    <t>crushed_wolframite</t>
+  </si>
+  <si>
+    <t>crushed_bauxite</t>
+  </si>
+  <si>
+    <t>crushed_netherrack</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials</t>
+  </si>
+  <si>
+    <t>forge:purified_materials</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/bauxite</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/copper</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/gold</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/iron</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/lead</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/netherrack</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/nickel</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/palladium</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/silver</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/stone</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/tin</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/wolframite</t>
+  </si>
+  <si>
+    <t>forge:crushed_materials/zinc</t>
+  </si>
+  <si>
+    <t>forge:purified_materials/copper</t>
+  </si>
+  <si>
+    <t>forge:purified_materials/gold</t>
+  </si>
+  <si>
+    <t>forge:purified_materials/iron</t>
+  </si>
+  <si>
+    <t>forge:purified_materials/lead</t>
+  </si>
+  <si>
+    <t>forge:purified_materials/nickel</t>
+  </si>
+  <si>
+    <t>forge:purified_materials/palladium</t>
+  </si>
+  <si>
+    <t>forge:purified_materials/silver</t>
+  </si>
+  <si>
+    <t>forge:purified_materials/tin</t>
+  </si>
+  <si>
+    <t>forge:purified_materials/zinc</t>
+  </si>
+  <si>
+    <t>raw_zinc_block</t>
+  </si>
+  <si>
+    <t>raw_lead_block</t>
+  </si>
+  <si>
+    <t>raw_nickel_block</t>
+  </si>
+  <si>
+    <t>raw_palladium_block</t>
+  </si>
+  <si>
+    <t>raw_tin_block</t>
+  </si>
+  <si>
+    <t>raw_silver_block</t>
+  </si>
+  <si>
+    <t>forge:storage_blocks/raw_zinc</t>
+  </si>
+  <si>
+    <t>forge:storage_blocks/raw_lead</t>
+  </si>
+  <si>
+    <t>forge:storage_blocks/raw_nickel</t>
+  </si>
+  <si>
+    <t>forge:storage_blocks/raw_palladium</t>
+  </si>
+  <si>
+    <t>forge:storage_blocks/raw_tin</t>
+  </si>
+  <si>
+    <t>forge:storage_blocks/raw_silver</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="M37" sqref="M36:O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1383,10 @@
     <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" customWidth="1"/>
+    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -1271,6 +1451,15 @@
       <c r="K4" t="s">
         <v>188</v>
       </c>
+      <c r="M4" t="s">
+        <v>292</v>
+      </c>
+      <c r="N4" t="s">
+        <v>294</v>
+      </c>
+      <c r="O4" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1300,6 +1489,15 @@
       <c r="K5" t="s">
         <v>189</v>
       </c>
+      <c r="M5" t="s">
+        <v>287</v>
+      </c>
+      <c r="N5" t="s">
+        <v>294</v>
+      </c>
+      <c r="O5" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -1329,6 +1527,15 @@
       <c r="K6" t="s">
         <v>190</v>
       </c>
+      <c r="M6" t="s">
+        <v>276</v>
+      </c>
+      <c r="N6" t="s">
+        <v>294</v>
+      </c>
+      <c r="O6" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1358,6 +1565,15 @@
       <c r="K7" t="s">
         <v>191</v>
       </c>
+      <c r="M7" t="s">
+        <v>285</v>
+      </c>
+      <c r="N7" t="s">
+        <v>294</v>
+      </c>
+      <c r="O7" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1387,6 +1603,15 @@
       <c r="K8" t="s">
         <v>192</v>
       </c>
+      <c r="M8" t="s">
+        <v>274</v>
+      </c>
+      <c r="N8" t="s">
+        <v>294</v>
+      </c>
+      <c r="O8" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -1416,6 +1641,15 @@
       <c r="K9" t="s">
         <v>193</v>
       </c>
+      <c r="M9" t="s">
+        <v>278</v>
+      </c>
+      <c r="N9" t="s">
+        <v>294</v>
+      </c>
+      <c r="O9" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1445,6 +1679,15 @@
       <c r="K10" t="s">
         <v>194</v>
       </c>
+      <c r="M10" t="s">
+        <v>293</v>
+      </c>
+      <c r="N10" t="s">
+        <v>294</v>
+      </c>
+      <c r="O10" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1474,6 +1717,15 @@
       <c r="K11" t="s">
         <v>195</v>
       </c>
+      <c r="M11" t="s">
+        <v>279</v>
+      </c>
+      <c r="N11" t="s">
+        <v>294</v>
+      </c>
+      <c r="O11" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1503,6 +1755,15 @@
       <c r="K12" t="s">
         <v>196</v>
       </c>
+      <c r="M12" t="s">
+        <v>281</v>
+      </c>
+      <c r="N12" t="s">
+        <v>294</v>
+      </c>
+      <c r="O12" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1532,6 +1793,15 @@
       <c r="K13" t="s">
         <v>197</v>
       </c>
+      <c r="M13" t="s">
+        <v>289</v>
+      </c>
+      <c r="N13" t="s">
+        <v>294</v>
+      </c>
+      <c r="O13" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -1561,6 +1831,15 @@
       <c r="K14" t="s">
         <v>198</v>
       </c>
+      <c r="M14" t="s">
+        <v>271</v>
+      </c>
+      <c r="N14" t="s">
+        <v>294</v>
+      </c>
+      <c r="O14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1590,6 +1869,15 @@
       <c r="K15" t="s">
         <v>199</v>
       </c>
+      <c r="M15" t="s">
+        <v>283</v>
+      </c>
+      <c r="N15" t="s">
+        <v>294</v>
+      </c>
+      <c r="O15" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1619,8 +1907,17 @@
       <c r="K16" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>291</v>
+      </c>
+      <c r="N16" t="s">
+        <v>294</v>
+      </c>
+      <c r="O16" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>19</v>
       </c>
@@ -1648,8 +1945,17 @@
       <c r="K17" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>272</v>
+      </c>
+      <c r="N17" t="s">
+        <v>294</v>
+      </c>
+      <c r="O17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -1677,8 +1983,17 @@
       <c r="K18" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>288</v>
+      </c>
+      <c r="N18" t="s">
+        <v>295</v>
+      </c>
+      <c r="O18" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>29</v>
       </c>
@@ -1706,8 +2021,17 @@
       <c r="K19" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>277</v>
+      </c>
+      <c r="N19" t="s">
+        <v>295</v>
+      </c>
+      <c r="O19" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>30</v>
       </c>
@@ -1735,8 +2059,17 @@
       <c r="K20" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>286</v>
+      </c>
+      <c r="N20" t="s">
+        <v>295</v>
+      </c>
+      <c r="O20" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -1764,8 +2097,17 @@
       <c r="K21" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>275</v>
+      </c>
+      <c r="N21" t="s">
+        <v>295</v>
+      </c>
+      <c r="O21" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>33</v>
       </c>
@@ -1793,8 +2135,17 @@
       <c r="K22" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>280</v>
+      </c>
+      <c r="N22" t="s">
+        <v>295</v>
+      </c>
+      <c r="O22" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>35</v>
       </c>
@@ -1822,8 +2173,17 @@
       <c r="K23" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>282</v>
+      </c>
+      <c r="N23" t="s">
+        <v>295</v>
+      </c>
+      <c r="O23" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>36</v>
       </c>
@@ -1851,8 +2211,17 @@
       <c r="K24" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>290</v>
+      </c>
+      <c r="N24" t="s">
+        <v>295</v>
+      </c>
+      <c r="O24" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>37</v>
       </c>
@@ -1880,8 +2249,17 @@
       <c r="K25" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>284</v>
+      </c>
+      <c r="N25" t="s">
+        <v>295</v>
+      </c>
+      <c r="O25" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>38</v>
       </c>
@@ -1909,8 +2287,17 @@
       <c r="K26" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>273</v>
+      </c>
+      <c r="N26" t="s">
+        <v>295</v>
+      </c>
+      <c r="O26" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>39</v>
       </c>
@@ -1939,7 +2326,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>43</v>
       </c>
@@ -1968,7 +2355,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>44</v>
       </c>
@@ -1997,7 +2384,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>45</v>
       </c>
@@ -2026,7 +2413,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>46</v>
       </c>
@@ -2055,7 +2442,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>55</v>
       </c>
@@ -2084,7 +2471,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>60</v>
       </c>
@@ -2113,7 +2500,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>71</v>
       </c>
@@ -2142,7 +2529,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>72</v>
       </c>
@@ -2171,7 +2558,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>73</v>
       </c>
@@ -2200,7 +2587,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>74</v>
       </c>
@@ -2228,8 +2615,15 @@
       <c r="K37" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M37" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="O37" s="3"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>75</v>
       </c>
@@ -2257,8 +2651,14 @@
       <c r="K38" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>318</v>
+      </c>
+      <c r="N38" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>77</v>
       </c>
@@ -2286,8 +2686,14 @@
       <c r="K39" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>319</v>
+      </c>
+      <c r="N39" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>78</v>
       </c>
@@ -2315,8 +2721,14 @@
       <c r="K40" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>320</v>
+      </c>
+      <c r="N40" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>76</v>
       </c>
@@ -2344,8 +2756,14 @@
       <c r="K41" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>321</v>
+      </c>
+      <c r="N41" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>79</v>
       </c>
@@ -2373,8 +2791,14 @@
       <c r="K42" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>322</v>
+      </c>
+      <c r="N42" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>80</v>
       </c>
@@ -2402,8 +2826,14 @@
       <c r="K43" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>323</v>
+      </c>
+      <c r="N43" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>81</v>
       </c>
@@ -2432,7 +2862,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>82</v>
       </c>
@@ -2461,7 +2891,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>83</v>
       </c>
@@ -2490,7 +2920,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>84</v>
       </c>
@@ -2519,7 +2949,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>85</v>
       </c>
@@ -3793,12 +4223,13 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="I51:J84">
-    <sortCondition ref="J75:J108"/>
+  <sortState ref="M4:M26">
+    <sortCondition ref="M6"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N37:O37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Loottables + FVH Verbessert
</commit_message>
<xml_diff>
--- a/Versandordner/Assets (technisch)/Liste Metallblockwerte.xlsx
+++ b/Versandordner/Assets (technisch)/Liste Metallblockwerte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="376">
   <si>
     <t>BLOCK</t>
   </si>
@@ -1014,6 +1014,144 @@
   </si>
   <si>
     <t>forge:storage_blocks/raw_silver</t>
+  </si>
+  <si>
+    <t>insulated_copper_wire_coil</t>
+  </si>
+  <si>
+    <t>insulated_tin_wire_coil</t>
+  </si>
+  <si>
+    <t>insulated_aluminum_wire_coil</t>
+  </si>
+  <si>
+    <t>copper_wire_coil</t>
+  </si>
+  <si>
+    <t>tin_wire_coil</t>
+  </si>
+  <si>
+    <t>aluminum_wire_coil</t>
+  </si>
+  <si>
+    <t>insulated_copper_wire</t>
+  </si>
+  <si>
+    <t>insulated_tin_wire</t>
+  </si>
+  <si>
+    <t>insulated_aluminum_wire</t>
+  </si>
+  <si>
+    <t>copper_wire</t>
+  </si>
+  <si>
+    <t>tin_wire</t>
+  </si>
+  <si>
+    <t>aluminum_wire</t>
+  </si>
+  <si>
+    <t>tin_wire_holder</t>
+  </si>
+  <si>
+    <t>iron_wire_holder</t>
+  </si>
+  <si>
+    <t>gold_wire_holder</t>
+  </si>
+  <si>
+    <t>aluminum_wire_holder</t>
+  </si>
+  <si>
+    <t>gold_wire</t>
+  </si>
+  <si>
+    <t>insulated_gold_wire</t>
+  </si>
+  <si>
+    <t>gold_wire_coil</t>
+  </si>
+  <si>
+    <t>insulated_gold_wire_coil</t>
+  </si>
+  <si>
+    <t>iron_junction_box</t>
+  </si>
+  <si>
+    <t>zinc_junction_box</t>
+  </si>
+  <si>
+    <t>brass_junction_box</t>
+  </si>
+  <si>
+    <t>steel_junction_box</t>
+  </si>
+  <si>
+    <t>brass_floodlight</t>
+  </si>
+  <si>
+    <t>steel_floodlight</t>
+  </si>
+  <si>
+    <t>portable_coal_generator</t>
+  </si>
+  <si>
+    <t>portable_fuel_generator</t>
+  </si>
+  <si>
+    <t>industriacore:electrics</t>
+  </si>
+  <si>
+    <t>industria:wire_holders</t>
+  </si>
+  <si>
+    <t>forge:wires</t>
+  </si>
+  <si>
+    <t>forge:wires/copper</t>
+  </si>
+  <si>
+    <t>forge:wires/tin</t>
+  </si>
+  <si>
+    <t>forge:wires/gold</t>
+  </si>
+  <si>
+    <t>forge:wires/aluminum</t>
+  </si>
+  <si>
+    <t>industriacore:conduits</t>
+  </si>
+  <si>
+    <t>industriacore:machinery</t>
+  </si>
+  <si>
+    <t>wire_holder</t>
+  </si>
+  <si>
+    <t>wire_coil</t>
+  </si>
+  <si>
+    <t>empty_coil</t>
+  </si>
+  <si>
+    <t>junction_box</t>
+  </si>
+  <si>
+    <t>floodlight</t>
+  </si>
+  <si>
+    <t>machines</t>
+  </si>
+  <si>
+    <t>axe</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>empty_wire_coil</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1078,18 +1216,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -1371,22 +1526,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O94"/>
+  <dimension ref="B3:R116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="M37" sqref="M36:O37"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" customWidth="1"/>
     <col min="13" max="13" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="31.42578125" customWidth="1"/>
     <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -2978,7 +3133,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>86</v>
       </c>
@@ -3006,8 +3161,17 @@
       <c r="K49" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M49" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="N49" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>15</v>
       </c>
@@ -3035,8 +3199,17 @@
       <c r="K50" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M50" t="s">
+        <v>330</v>
+      </c>
+      <c r="N50" t="s">
+        <v>358</v>
+      </c>
+      <c r="O50" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>42</v>
       </c>
@@ -3064,8 +3237,17 @@
       <c r="K51" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M51" t="s">
+        <v>331</v>
+      </c>
+      <c r="N51" t="s">
+        <v>358</v>
+      </c>
+      <c r="O51" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>6</v>
       </c>
@@ -3093,8 +3275,17 @@
       <c r="K52" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M52" t="s">
+        <v>349</v>
+      </c>
+      <c r="N52" t="s">
+        <v>358</v>
+      </c>
+      <c r="O52" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>20</v>
       </c>
@@ -3122,8 +3313,17 @@
       <c r="K53" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M53" t="s">
+        <v>332</v>
+      </c>
+      <c r="N53" t="s">
+        <v>358</v>
+      </c>
+      <c r="O53" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>21</v>
       </c>
@@ -3151,8 +3351,17 @@
       <c r="K54" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M54" t="s">
+        <v>333</v>
+      </c>
+      <c r="N54" t="s">
+        <v>358</v>
+      </c>
+      <c r="O54" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>22</v>
       </c>
@@ -3180,8 +3389,17 @@
       <c r="K55" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M55" t="s">
+        <v>334</v>
+      </c>
+      <c r="N55" t="s">
+        <v>358</v>
+      </c>
+      <c r="O55" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>23</v>
       </c>
@@ -3209,8 +3427,17 @@
       <c r="K56" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M56" t="s">
+        <v>348</v>
+      </c>
+      <c r="N56" t="s">
+        <v>358</v>
+      </c>
+      <c r="O56" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>25</v>
       </c>
@@ -3238,8 +3465,17 @@
       <c r="K57" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M57" t="s">
+        <v>335</v>
+      </c>
+      <c r="N57" t="s">
+        <v>358</v>
+      </c>
+      <c r="O57" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>26</v>
       </c>
@@ -3267,8 +3503,17 @@
       <c r="K58" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M58" t="s">
+        <v>336</v>
+      </c>
+      <c r="N58" t="s">
+        <v>358</v>
+      </c>
+      <c r="O58" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>27</v>
       </c>
@@ -3296,8 +3541,17 @@
       <c r="K59" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M59" t="s">
+        <v>337</v>
+      </c>
+      <c r="N59" t="s">
+        <v>358</v>
+      </c>
+      <c r="O59" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>28</v>
       </c>
@@ -3325,8 +3579,17 @@
       <c r="K60" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M60" t="s">
+        <v>347</v>
+      </c>
+      <c r="N60" t="s">
+        <v>358</v>
+      </c>
+      <c r="O60" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>31</v>
       </c>
@@ -3354,8 +3617,17 @@
       <c r="K61" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M61" t="s">
+        <v>338</v>
+      </c>
+      <c r="N61" t="s">
+        <v>358</v>
+      </c>
+      <c r="O61" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>41</v>
       </c>
@@ -3383,8 +3655,23 @@
       <c r="K62" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M62" t="s">
+        <v>339</v>
+      </c>
+      <c r="N62" t="s">
+        <v>358</v>
+      </c>
+      <c r="O62" t="s">
+        <v>365</v>
+      </c>
+      <c r="P62" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>47</v>
       </c>
@@ -3412,8 +3699,23 @@
       <c r="K63" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M63" t="s">
+        <v>340</v>
+      </c>
+      <c r="N63" t="s">
+        <v>358</v>
+      </c>
+      <c r="O63" t="s">
+        <v>365</v>
+      </c>
+      <c r="P63" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>48</v>
       </c>
@@ -3441,8 +3743,23 @@
       <c r="K64" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M64" t="s">
+        <v>346</v>
+      </c>
+      <c r="N64" t="s">
+        <v>358</v>
+      </c>
+      <c r="O64" t="s">
+        <v>365</v>
+      </c>
+      <c r="P64" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>49</v>
       </c>
@@ -3470,8 +3787,23 @@
       <c r="K65" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M65" t="s">
+        <v>341</v>
+      </c>
+      <c r="N65" t="s">
+        <v>358</v>
+      </c>
+      <c r="O65" t="s">
+        <v>365</v>
+      </c>
+      <c r="P65" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>50</v>
       </c>
@@ -3499,8 +3831,17 @@
       <c r="K66" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M66" t="s">
+        <v>342</v>
+      </c>
+      <c r="N66" t="s">
+        <v>358</v>
+      </c>
+      <c r="O66" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>51</v>
       </c>
@@ -3528,8 +3869,17 @@
       <c r="K67" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M67" t="s">
+        <v>343</v>
+      </c>
+      <c r="N67" t="s">
+        <v>358</v>
+      </c>
+      <c r="O67" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>52</v>
       </c>
@@ -3557,8 +3907,17 @@
       <c r="K68" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M68" t="s">
+        <v>344</v>
+      </c>
+      <c r="N68" t="s">
+        <v>358</v>
+      </c>
+      <c r="O68" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>53</v>
       </c>
@@ -3586,8 +3945,17 @@
       <c r="K69" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M69" t="s">
+        <v>345</v>
+      </c>
+      <c r="N69" t="s">
+        <v>358</v>
+      </c>
+      <c r="O69" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>54</v>
       </c>
@@ -3615,8 +3983,17 @@
       <c r="K70" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M70" t="s">
+        <v>350</v>
+      </c>
+      <c r="N70" t="s">
+        <v>358</v>
+      </c>
+      <c r="O70" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>56</v>
       </c>
@@ -3644,8 +4021,17 @@
       <c r="K71" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M71" t="s">
+        <v>351</v>
+      </c>
+      <c r="N71" t="s">
+        <v>358</v>
+      </c>
+      <c r="O71" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>57</v>
       </c>
@@ -3673,8 +4059,17 @@
       <c r="K72" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M72" t="s">
+        <v>352</v>
+      </c>
+      <c r="N72" t="s">
+        <v>358</v>
+      </c>
+      <c r="O72" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>58</v>
       </c>
@@ -3702,8 +4097,17 @@
       <c r="K73" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M73" t="s">
+        <v>353</v>
+      </c>
+      <c r="N73" t="s">
+        <v>358</v>
+      </c>
+      <c r="O73" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>59</v>
       </c>
@@ -3731,8 +4135,17 @@
       <c r="K74" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M74" t="s">
+        <v>354</v>
+      </c>
+      <c r="N74" t="s">
+        <v>358</v>
+      </c>
+      <c r="O74" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>65</v>
       </c>
@@ -3760,8 +4173,17 @@
       <c r="K75" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M75" t="s">
+        <v>355</v>
+      </c>
+      <c r="N75" t="s">
+        <v>358</v>
+      </c>
+      <c r="O75" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>66</v>
       </c>
@@ -3789,8 +4211,17 @@
       <c r="K76" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M76" t="s">
+        <v>356</v>
+      </c>
+      <c r="N76" t="s">
+        <v>358</v>
+      </c>
+      <c r="O76" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>67</v>
       </c>
@@ -3818,8 +4249,17 @@
       <c r="K77" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M77" t="s">
+        <v>357</v>
+      </c>
+      <c r="N77" t="s">
+        <v>358</v>
+      </c>
+      <c r="O77" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>68</v>
       </c>
@@ -3848,7 +4288,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>69</v>
       </c>
@@ -3877,7 +4317,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>99</v>
       </c>
@@ -3906,7 +4346,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>100</v>
       </c>
@@ -3935,7 +4375,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>70</v>
       </c>
@@ -3964,7 +4404,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>87</v>
       </c>
@@ -3993,7 +4433,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>88</v>
       </c>
@@ -4021,8 +4461,26 @@
       <c r="K84" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N84" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O84" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P84" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R84" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>89</v>
       </c>
@@ -4041,8 +4499,26 @@
       <c r="G85" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M85" t="s">
+        <v>367</v>
+      </c>
+      <c r="N85" s="7">
+        <v>4</v>
+      </c>
+      <c r="O85">
+        <v>4</v>
+      </c>
+      <c r="P85">
+        <v>30</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>61</v>
+      </c>
+      <c r="R85" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>90</v>
       </c>
@@ -4061,8 +4537,26 @@
       <c r="G86" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M86" t="s">
+        <v>368</v>
+      </c>
+      <c r="N86" s="7">
+        <v>4</v>
+      </c>
+      <c r="O86">
+        <v>4</v>
+      </c>
+      <c r="P86">
+        <v>4000</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>373</v>
+      </c>
+      <c r="R86" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="87" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>91</v>
       </c>
@@ -4081,8 +4575,26 @@
       <c r="G87" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M87" t="s">
+        <v>369</v>
+      </c>
+      <c r="N87" s="7">
+        <v>3</v>
+      </c>
+      <c r="O87">
+        <v>3</v>
+      </c>
+      <c r="P87">
+        <v>600</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>373</v>
+      </c>
+      <c r="R87" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="88" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>92</v>
       </c>
@@ -4101,8 +4613,26 @@
       <c r="G88" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M88" t="s">
+        <v>370</v>
+      </c>
+      <c r="N88" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="O88">
+        <v>0.4</v>
+      </c>
+      <c r="P88">
+        <v>20</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>61</v>
+      </c>
+      <c r="R88" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>93</v>
       </c>
@@ -4121,8 +4651,26 @@
       <c r="G89" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M89" t="s">
+        <v>371</v>
+      </c>
+      <c r="N89" s="7">
+        <v>1</v>
+      </c>
+      <c r="O89">
+        <v>1</v>
+      </c>
+      <c r="P89">
+        <v>900</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>61</v>
+      </c>
+      <c r="R89" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>94</v>
       </c>
@@ -4141,8 +4689,26 @@
       <c r="G90" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M90" t="s">
+        <v>372</v>
+      </c>
+      <c r="N90" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="O90">
+        <v>3.5</v>
+      </c>
+      <c r="P90">
+        <v>1500</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>61</v>
+      </c>
+      <c r="R90" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>95</v>
       </c>
@@ -4162,7 +4728,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>96</v>
       </c>
@@ -4182,7 +4748,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>97</v>
       </c>
@@ -4202,7 +4768,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>98</v>
       </c>
@@ -4220,16 +4786,185 @@
       </c>
       <c r="G94" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="96" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="M96" t="s">
+        <v>330</v>
+      </c>
+      <c r="N96">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="97" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M97" t="s">
+        <v>331</v>
+      </c>
+      <c r="N97">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="98" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M98" t="s">
+        <v>349</v>
+      </c>
+      <c r="N98">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="99" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M99" t="s">
+        <v>332</v>
+      </c>
+      <c r="N99">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="100" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M100" t="s">
+        <v>333</v>
+      </c>
+      <c r="N100">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="101" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M101" t="s">
+        <v>334</v>
+      </c>
+      <c r="N101">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="102" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M102" t="s">
+        <v>348</v>
+      </c>
+      <c r="N102">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="103" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M103" t="s">
+        <v>335</v>
+      </c>
+      <c r="N103">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="104" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M104" t="s">
+        <v>375</v>
+      </c>
+      <c r="N104">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="105" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M105" t="s">
+        <v>342</v>
+      </c>
+      <c r="N105">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="106" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M106" t="s">
+        <v>343</v>
+      </c>
+      <c r="N106">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M107" t="s">
+        <v>344</v>
+      </c>
+      <c r="N107">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="108" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M108" t="s">
+        <v>345</v>
+      </c>
+      <c r="N108">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="109" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M109" t="s">
+        <v>350</v>
+      </c>
+      <c r="N109">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M110" t="s">
+        <v>351</v>
+      </c>
+      <c r="N110">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M111" t="s">
+        <v>352</v>
+      </c>
+      <c r="N111">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M112" t="s">
+        <v>353</v>
+      </c>
+      <c r="N112">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M113" t="s">
+        <v>354</v>
+      </c>
+      <c r="N113">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="114" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M114" t="s">
+        <v>355</v>
+      </c>
+      <c r="N114">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="115" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M115" t="s">
+        <v>356</v>
+      </c>
+      <c r="N115">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="116" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M116" t="s">
+        <v>357</v>
+      </c>
+      <c r="N116">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="M4:M26">
     <sortCondition ref="M6"/>
   </sortState>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N49:Q49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>